<commit_message>
Corregir cálculos de strings según leyes eléctricas
FIX CRÍTICO: Cálculos de strings corregidos

CONEXIÓN EN SERIE:
✅ Voltaje: Vmp × Paneles (SE SUMAN los voltajes)
✅ Corriente: Imp (SE MANTIENE la corriente)
✅ Potencia: Pmax × Paneles (SE SUMA)

Ejemplo: 2 paneles 400W (36.5V, 10.96A) en serie
  V = 36.5V × 2 = 73V
  I = 10.96A (mantiene)
  P = 400W × 2 = 800W

CONEXIÓN EN PARALELO:
✅ Voltaje: Vmp (SE MANTIENE el voltaje)
✅ Corriente: Imp × Paneles (SE SUMAN las corrientes)
✅ Potencia: Pmax × Paneles (SE SUMA)

Ejemplo: 2 paneles 400W (36.5V, 10.96A) en paralelo
  V = 36.5V (mantiene)
  I = 10.96A × 2 = 21.92A
  P = 400W × 2 = 800W

PRINCIPIO FUNDAMENTAL:
⚡ LA POTENCIA SIEMPRE SE SUMA independientemente
   de si es serie, paralelo o serie-paralelo

Fórmulas actualizadas según leyes de Kirchhoff
</commit_message>
<xml_diff>
--- a/calculadora_solar/Calculadora_Solar_V4.1_Completa.xlsx
+++ b/calculadora_solar/Calculadora_Solar_V4.1_Completa.xlsx
@@ -1832,7 +1832,7 @@
       </c>
       <c r="C40" s="37" t="n"/>
       <c r="D40" s="21">
-        <f>IF(D36="Serie",D34*D37,IF(D36="Paralelo",D34,D34*SQRT(D37)))</f>
+        <f>IF(D36="Serie",D34*D37,IF(D36="Paralelo",D34,"N/A"))</f>
         <v/>
       </c>
       <c r="E40" s="4" t="inlineStr">
@@ -1842,7 +1842,7 @@
       </c>
       <c r="F40" s="9" t="inlineStr">
         <is>
-          <t>Vmp × Paneles (serie) o Vmp (paralelo)</t>
+          <t>Serie: V×Paneles | Paralelo: V</t>
         </is>
       </c>
       <c r="G40" s="36" t="n"/>
@@ -1858,7 +1858,7 @@
       </c>
       <c r="C41" s="37" t="n"/>
       <c r="D41" s="21">
-        <f>IF(D36="Serie",D35,IF(D36="Paralelo",D35*D37,D35*SQRT(D37)))</f>
+        <f>IF(D36="Serie",D35,IF(D36="Paralelo",D35*D37,"N/A"))</f>
         <v/>
       </c>
       <c r="E41" s="4" t="inlineStr">
@@ -1868,7 +1868,7 @@
       </c>
       <c r="F41" s="9" t="inlineStr">
         <is>
-          <t>Imp (serie) o Imp × Paneles (paralelo)</t>
+          <t>Serie: I | Paralelo: I×Paneles</t>
         </is>
       </c>
       <c r="G41" s="36" t="n"/>
@@ -1884,7 +1884,7 @@
       </c>
       <c r="C42" s="37" t="n"/>
       <c r="D42" s="21">
-        <f>D40*D41</f>
+        <f>D33*D37</f>
         <v/>
       </c>
       <c r="E42" s="4" t="inlineStr">
@@ -1894,7 +1894,7 @@
       </c>
       <c r="F42" s="9" t="inlineStr">
         <is>
-          <t>Vstring × Istring</t>
+          <t>SIEMPRE: P×Paneles (se suma)</t>
         </is>
       </c>
       <c r="G42" s="36" t="n"/>
@@ -2620,7 +2620,6 @@
         <v/>
       </c>
     </row>
-    <row r="15"/>
     <row r="16">
       <c r="A16" s="34" t="inlineStr">
         <is>
@@ -4037,6 +4036,12 @@
           <t>SUBTOTAL PANELES SOLARES</t>
         </is>
       </c>
+      <c r="B38" s="36" t="n"/>
+      <c r="C38" s="36" t="n"/>
+      <c r="D38" s="36" t="n"/>
+      <c r="E38" s="36" t="n"/>
+      <c r="F38" s="36" t="n"/>
+      <c r="G38" s="37" t="n"/>
       <c r="H38" s="49">
         <f>SUM(H5:H8)</f>
         <v/>
@@ -4048,6 +4053,12 @@
           <t>SUBTOTAL INVERSOR</t>
         </is>
       </c>
+      <c r="B39" s="36" t="n"/>
+      <c r="C39" s="36" t="n"/>
+      <c r="D39" s="36" t="n"/>
+      <c r="E39" s="36" t="n"/>
+      <c r="F39" s="36" t="n"/>
+      <c r="G39" s="37" t="n"/>
       <c r="H39" s="49">
         <f>SUM(H9:H10)</f>
         <v/>
@@ -4059,6 +4070,12 @@
           <t>SUBTOTAL BATERÍAS</t>
         </is>
       </c>
+      <c r="B40" s="36" t="n"/>
+      <c r="C40" s="36" t="n"/>
+      <c r="D40" s="36" t="n"/>
+      <c r="E40" s="36" t="n"/>
+      <c r="F40" s="36" t="n"/>
+      <c r="G40" s="37" t="n"/>
       <c r="H40" s="49">
         <f>SUM(H11:H13)</f>
         <v/>
@@ -4070,6 +4087,12 @@
           <t>SUBTOTAL CABLEADO DC</t>
         </is>
       </c>
+      <c r="B41" s="36" t="n"/>
+      <c r="C41" s="36" t="n"/>
+      <c r="D41" s="36" t="n"/>
+      <c r="E41" s="36" t="n"/>
+      <c r="F41" s="36" t="n"/>
+      <c r="G41" s="37" t="n"/>
       <c r="H41" s="49">
         <f>SUM(H14:H17)</f>
         <v/>
@@ -4081,6 +4104,12 @@
           <t>SUBTOTAL CABLEADO AC</t>
         </is>
       </c>
+      <c r="B42" s="36" t="n"/>
+      <c r="C42" s="36" t="n"/>
+      <c r="D42" s="36" t="n"/>
+      <c r="E42" s="36" t="n"/>
+      <c r="F42" s="36" t="n"/>
+      <c r="G42" s="37" t="n"/>
       <c r="H42" s="49">
         <f>SUM(H18:H20)</f>
         <v/>
@@ -4092,6 +4121,12 @@
           <t>SUBTOTAL PROTECCIONES</t>
         </is>
       </c>
+      <c r="B43" s="36" t="n"/>
+      <c r="C43" s="36" t="n"/>
+      <c r="D43" s="36" t="n"/>
+      <c r="E43" s="36" t="n"/>
+      <c r="F43" s="36" t="n"/>
+      <c r="G43" s="37" t="n"/>
       <c r="H43" s="49">
         <f>SUM(H21:H25)</f>
         <v/>
@@ -4103,6 +4138,12 @@
           <t>SUBTOTAL TABLEROS</t>
         </is>
       </c>
+      <c r="B44" s="36" t="n"/>
+      <c r="C44" s="36" t="n"/>
+      <c r="D44" s="36" t="n"/>
+      <c r="E44" s="36" t="n"/>
+      <c r="F44" s="36" t="n"/>
+      <c r="G44" s="37" t="n"/>
       <c r="H44" s="49">
         <f>SUM(H26:H28)</f>
         <v/>
@@ -4114,6 +4155,12 @@
           <t>SUBTOTAL PUESTA A TIERRA</t>
         </is>
       </c>
+      <c r="B45" s="36" t="n"/>
+      <c r="C45" s="36" t="n"/>
+      <c r="D45" s="36" t="n"/>
+      <c r="E45" s="36" t="n"/>
+      <c r="F45" s="36" t="n"/>
+      <c r="G45" s="37" t="n"/>
       <c r="H45" s="49">
         <f>SUM(H29:H31)</f>
         <v/>
@@ -4125,6 +4172,12 @@
           <t>SUBTOTAL MATERIALES VARIOS</t>
         </is>
       </c>
+      <c r="B46" s="36" t="n"/>
+      <c r="C46" s="36" t="n"/>
+      <c r="D46" s="36" t="n"/>
+      <c r="E46" s="36" t="n"/>
+      <c r="F46" s="36" t="n"/>
+      <c r="G46" s="37" t="n"/>
       <c r="H46" s="49">
         <f>SUM(H32:H36)</f>
         <v/>
@@ -4136,6 +4189,12 @@
           <t>TOTAL MATERIALES Y COMPONENTES</t>
         </is>
       </c>
+      <c r="B48" s="36" t="n"/>
+      <c r="C48" s="36" t="n"/>
+      <c r="D48" s="36" t="n"/>
+      <c r="E48" s="36" t="n"/>
+      <c r="F48" s="36" t="n"/>
+      <c r="G48" s="37" t="n"/>
       <c r="H48" s="51">
         <f>SUM(H5:H36)</f>
         <v/>
@@ -4147,6 +4206,12 @@
           <t>MANO DE OBRA INSTALACIÓN</t>
         </is>
       </c>
+      <c r="B49" s="36" t="n"/>
+      <c r="C49" s="36" t="n"/>
+      <c r="D49" s="36" t="n"/>
+      <c r="E49" s="36" t="n"/>
+      <c r="F49" s="36" t="n"/>
+      <c r="G49" s="37" t="n"/>
       <c r="H49" s="53" t="n">
         <v>2500</v>
       </c>
@@ -4157,6 +4222,12 @@
           <t>💵 INVERSIÓN TOTAL DEL PROYECTO</t>
         </is>
       </c>
+      <c r="B50" s="36" t="n"/>
+      <c r="C50" s="36" t="n"/>
+      <c r="D50" s="36" t="n"/>
+      <c r="E50" s="36" t="n"/>
+      <c r="F50" s="36" t="n"/>
+      <c r="G50" s="37" t="n"/>
       <c r="H50" s="55">
         <f>H48+H49</f>
         <v/>

</xml_diff>

<commit_message>
Fix: Corregir todas las referencias en hoja Informe Cliente
CORRECCIÓN DE REFERENCIAS EN INFORME:

Todas las fórmulas ahora apuntan a las filas correctas:
✅ D27 = Voltaje del sistema
✅ D28 = Frecuencia
✅ D29 = Tipo de red
✅ D30 = Tipo de inversor
✅ D33 = Potencia panel (Pmax)
✅ D36 = Configuración string
✅ D37 = Paneles por string
✅ D40 = Voltaje del string
✅ D41 = Corriente del string
✅ D46 = Tipo de batería
✅ D53 = Consumo diario real
✅ D56 = Capacidad banco (Ah)
✅ D58 = Potencia recomendada
✅ D59 = Cantidad paneles
✅ D60 = Número de strings
✅ D61 = Potencia del inversor
✅ D62 = Corriente controlador

Ahora el informe muestra los datos correctos de la Calculadora
</commit_message>
<xml_diff>
--- a/calculadora_solar/Calculadora_Solar_V4.1_Completa.xlsx
+++ b/calculadora_solar/Calculadora_Solar_V4.1_Completa.xlsx
@@ -2620,6 +2620,7 @@
         <v/>
       </c>
     </row>
+    <row r="15"/>
     <row r="16">
       <c r="A16" s="34" t="inlineStr">
         <is>
@@ -2645,7 +2646,7 @@
         </is>
       </c>
       <c r="B18" s="33">
-        <f>TEXT(Calculadora!D63,"0.00")&amp;" Wp"</f>
+        <f>TEXT(Calculadora!D58,"0.00")&amp;" Wp"</f>
         <v/>
       </c>
     </row>
@@ -2656,7 +2657,7 @@
         </is>
       </c>
       <c r="B19" s="33">
-        <f>Calculadora!D64&amp;" paneles de "&amp;TEXT(Calculadora!D34,"0.00")&amp;"W"</f>
+        <f>Calculadora!D59&amp;" paneles de "&amp;TEXT(Calculadora!D33,"0.00")&amp;"W"</f>
         <v/>
       </c>
     </row>
@@ -2748,6 +2749,7 @@
         <v/>
       </c>
     </row>
+    <row r="28"/>
     <row r="29">
       <c r="A29" s="35" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Fix: Hacer strings editables y corregir lógica de paneles totales
CAMBIOS CRÍTICOS V4.1:

1. CÁLCULOS DE STRING AHORA EDITABLES:
   ✅ Voltaje del string (D40): EDITABLE según modelo inversor
   ✅ Corriente del string (D41): EDITABLE según modelo inversor
   ✅ Potencia del string (D42): EDITABLE

   Los valores dependen del inversor específico, por eso
   deben ser editables por el usuario

2. NUEVA FILA: Paneles totales reales (D61)
   Fórmula: =D60×D37

   Esta es la cantidad REAL de paneles a comprar

3. LÓGICA CORREGIDA:
   • D59 = Paneles necesarios (según potencia)
   • D37 = Paneles por string (editable)
   • D60 = Strings = ROUNDUP(D59/D37, 0)
   • D61 = Paneles REALES = D60 × D37

EJEMPLO:
Si necesita 18 paneles y configura 10 paneles/string:
  → Strings: ROUNDUP(18/10) = 2 strings
  → Paneles REALES: 2 × 10 = 20 paneles

Si configura 1 string con 10 paneles:
  → Strings: 1
  → Paneles REALES: 1 × 10 = 10 paneles

Referencias informe actualizadas a filas 62 y 63
</commit_message>
<xml_diff>
--- a/calculadora_solar/Calculadora_Solar_V4.1_Completa.xlsx
+++ b/calculadora_solar/Calculadora_Solar_V4.1_Completa.xlsx
@@ -260,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -405,6 +405,9 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="10" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -771,7 +774,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J64"/>
+  <dimension ref="A1:J65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1831,9 +1834,8 @@
         </is>
       </c>
       <c r="C40" s="37" t="n"/>
-      <c r="D40" s="21">
-        <f>IF(D36="Serie",D34*D37,IF(D36="Paralelo",D34,"N/A"))</f>
-        <v/>
+      <c r="D40" s="18" t="n">
+        <v>73</v>
       </c>
       <c r="E40" s="4" t="inlineStr">
         <is>
@@ -1842,7 +1844,7 @@
       </c>
       <c r="F40" s="9" t="inlineStr">
         <is>
-          <t>Serie: V×Paneles | Paralelo: V</t>
+          <t>EDITAR según modelo inversor</t>
         </is>
       </c>
       <c r="G40" s="36" t="n"/>
@@ -1857,9 +1859,8 @@
         </is>
       </c>
       <c r="C41" s="37" t="n"/>
-      <c r="D41" s="21">
-        <f>IF(D36="Serie",D35,IF(D36="Paralelo",D35*D37,"N/A"))</f>
-        <v/>
+      <c r="D41" s="18" t="n">
+        <v>10.96</v>
       </c>
       <c r="E41" s="4" t="inlineStr">
         <is>
@@ -1868,7 +1869,7 @@
       </c>
       <c r="F41" s="9" t="inlineStr">
         <is>
-          <t>Serie: I | Paralelo: I×Paneles</t>
+          <t>EDITAR según modelo inversor</t>
         </is>
       </c>
       <c r="G41" s="36" t="n"/>
@@ -1883,9 +1884,8 @@
         </is>
       </c>
       <c r="C42" s="37" t="n"/>
-      <c r="D42" s="21">
-        <f>D33*D37</f>
-        <v/>
+      <c r="D42" s="18" t="n">
+        <v>800</v>
       </c>
       <c r="E42" s="4" t="inlineStr">
         <is>
@@ -1894,7 +1894,7 @@
       </c>
       <c r="F42" s="9" t="inlineStr">
         <is>
-          <t>SIEMPRE: P×Paneles (se suma)</t>
+          <t>EDITAR según configuración</t>
         </is>
       </c>
       <c r="G42" s="36" t="n"/>
@@ -2306,7 +2306,7 @@
       </c>
       <c r="F60" s="9" t="inlineStr">
         <is>
-          <t>Según config.</t>
+          <t>Paneles necesarios / Paneles por string</t>
         </is>
       </c>
       <c r="G60" s="36" t="n"/>
@@ -2317,48 +2317,43 @@
     <row r="61">
       <c r="B61" s="15" t="inlineStr">
         <is>
-          <t>Potencia del inversor</t>
-        </is>
-      </c>
-      <c r="C61" s="37" t="n"/>
-      <c r="D61" s="21">
-        <f>MAX(D5:D22)*1.25</f>
+          <t>Paneles totales reales</t>
+        </is>
+      </c>
+      <c r="D61" s="57">
+        <f>D60*D37</f>
         <v/>
       </c>
       <c r="E61" s="4" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>unidades</t>
         </is>
       </c>
       <c r="F61" s="9" t="inlineStr">
         <is>
-          <t>Pico + 25%</t>
-        </is>
-      </c>
-      <c r="G61" s="36" t="n"/>
-      <c r="H61" s="36" t="n"/>
-      <c r="I61" s="36" t="n"/>
-      <c r="J61" s="37" t="n"/>
+          <t>Strings × Paneles/string = Total a comprar</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="B62" s="15" t="inlineStr">
         <is>
-          <t>Corriente controlador</t>
+          <t>Potencia del inversor</t>
         </is>
       </c>
       <c r="C62" s="37" t="n"/>
       <c r="D62" s="21">
-        <f>D58/D27*1.25</f>
+        <f>MAX(D5:D22)*1.25</f>
         <v/>
       </c>
       <c r="E62" s="4" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F62" s="9" t="inlineStr">
         <is>
-          <t>Con margen</t>
+          <t>Pico + 25%</t>
         </is>
       </c>
       <c r="G62" s="36" t="n"/>
@@ -2366,8 +2361,35 @@
       <c r="I62" s="36" t="n"/>
       <c r="J62" s="37" t="n"/>
     </row>
-    <row r="64" ht="35" customHeight="1">
-      <c r="A64" s="26" t="inlineStr">
+    <row r="63">
+      <c r="B63" s="15" t="inlineStr">
+        <is>
+          <t>Corriente controlador</t>
+        </is>
+      </c>
+      <c r="C63" s="37" t="n"/>
+      <c r="D63" s="21">
+        <f>D58/D27*1.25</f>
+        <v/>
+      </c>
+      <c r="E63" s="4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="F63" s="9" t="inlineStr">
+        <is>
+          <t>Con margen</t>
+        </is>
+      </c>
+      <c r="G63" s="36" t="n"/>
+      <c r="H63" s="36" t="n"/>
+      <c r="I63" s="36" t="n"/>
+      <c r="J63" s="37" t="n"/>
+    </row>
+    <row r="64" ht="35" customHeight="1"/>
+    <row r="65">
+      <c r="A65" s="26" t="inlineStr">
         <is>
           <t>📄 Para generar INFORME PDF: Vaya a la pestaña "Informe Cliente" y guarde como PDF desde Excel (Archivo → Guardar como → PDF)</t>
         </is>
@@ -2657,7 +2679,7 @@
         </is>
       </c>
       <c r="B19" s="33">
-        <f>Calculadora!D59&amp;" paneles de "&amp;TEXT(Calculadora!D33,"0.00")&amp;"W"</f>
+        <f>Calculadora!D61&amp;" paneles de "&amp;TEXT(Calculadora!D33,"0.00")&amp;"W"</f>
         <v/>
       </c>
     </row>
@@ -2712,7 +2734,7 @@
         </is>
       </c>
       <c r="B24" s="33">
-        <f>ROUND(Calculadora!D61/1000,1)&amp;" kW"</f>
+        <f>ROUND(Calculadora!D62/1000,1)&amp;" kW"</f>
         <v/>
       </c>
     </row>
@@ -2745,7 +2767,7 @@
         </is>
       </c>
       <c r="B27" s="33">
-        <f>ROUND(Calculadora!D62,0)&amp;" A"</f>
+        <f>ROUND(Calculadora!D63,0)&amp;" A"</f>
         <v/>
       </c>
     </row>

</xml_diff>